<commit_message>
updated the simplex datasets
</commit_message>
<xml_diff>
--- a/Airport_Label.xlsx
+++ b/Airport_Label.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yechixia/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{678BF52C-182E-134B-AF57-66132C10A118}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{57C01133-AB5A-1F4D-8304-9A913DC8B0C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15440" yWindow="1940" windowWidth="28100" windowHeight="16480" xr2:uid="{BFF24862-BE81-F743-A143-FC4B11EBC1C8}"/>
+    <workbookView xWindow="9640" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{BFF24862-BE81-F743-A143-FC4B11EBC1C8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -348,7 +348,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -370,6 +370,20 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="等线"/>
+      <family val="4"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -379,7 +393,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -389,16 +403,29 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
       </bottom>
       <diagonal/>
     </border>
@@ -415,13 +442,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -769,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5E3F2B1-3329-E74C-8FE9-AEE04699C9BE}">
-  <dimension ref="A1:E99"/>
+  <dimension ref="A1:E98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -796,203 +823,203 @@
     </row>
     <row r="2" spans="1:5">
       <c r="A2" s="2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B2" s="2">
+        <v>700</v>
+      </c>
+      <c r="C2" s="2">
         <v>100</v>
       </c>
-      <c r="C2" s="4">
-        <v>8</v>
-      </c>
-      <c r="D2" s="4">
-        <v>10</v>
-      </c>
-      <c r="E2" s="4">
-        <v>21</v>
+      <c r="D2" s="2">
+        <v>100</v>
+      </c>
+      <c r="E2" s="2">
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" s="4">
-        <v>100</v>
+        <v>101</v>
+      </c>
+      <c r="B3" s="2">
+        <v>750</v>
       </c>
       <c r="C3" s="2">
-        <v>8</v>
+        <v>150</v>
       </c>
       <c r="D3" s="2">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="E3" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4" s="2">
-        <v>50</v>
-      </c>
-      <c r="C4" s="4">
-        <v>8</v>
-      </c>
-      <c r="D4" s="4">
+        <v>57</v>
+      </c>
+      <c r="C4" s="2">
+        <v>3</v>
+      </c>
+      <c r="D4" s="3">
         <v>10</v>
       </c>
       <c r="E4" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B5" s="4">
-        <v>50</v>
+        <v>8</v>
+      </c>
+      <c r="B5" s="2">
+        <v>57</v>
       </c>
       <c r="C5" s="2">
-        <v>8</v>
-      </c>
-      <c r="D5" s="2">
+        <v>3</v>
+      </c>
+      <c r="D5" s="4">
         <v>10</v>
       </c>
       <c r="E5" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>24</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
-        <v>50</v>
-      </c>
-      <c r="C6" s="4">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="C6" s="2">
+        <v>4</v>
       </c>
       <c r="D6" s="4">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E6" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="4">
-        <v>50</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="2">
+        <v>57</v>
       </c>
       <c r="C7" s="2">
-        <v>8</v>
-      </c>
-      <c r="D7" s="2">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D7" s="4">
+        <v>10</v>
       </c>
       <c r="E7" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
-        <v>50</v>
-      </c>
-      <c r="C8" s="4">
-        <v>8</v>
+        <v>57</v>
+      </c>
+      <c r="C8" s="2">
+        <v>4</v>
       </c>
       <c r="D8" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E8" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9" s="4">
-        <v>50</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="2">
+        <v>57</v>
       </c>
       <c r="C9" s="2">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D9" s="4">
+        <v>10</v>
       </c>
       <c r="E9" s="2">
-        <v>17</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="B10" s="4">
-        <v>81</v>
-      </c>
-      <c r="C10" s="4">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="B10" s="2">
+        <v>57</v>
+      </c>
+      <c r="C10" s="2">
+        <v>4</v>
       </c>
       <c r="D10" s="4">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E10" s="2">
-        <v>19</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>73</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
-        <v>50</v>
+        <v>57</v>
       </c>
       <c r="C11" s="2">
-        <v>5</v>
-      </c>
-      <c r="D11" s="2">
-        <v>5</v>
+        <v>4</v>
+      </c>
+      <c r="D11" s="4">
+        <v>10</v>
       </c>
       <c r="E11" s="2">
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B12" s="4">
-        <v>50</v>
+        <v>15</v>
+      </c>
+      <c r="B12" s="2">
+        <v>57</v>
       </c>
       <c r="C12" s="2">
-        <v>21</v>
-      </c>
-      <c r="D12" s="2">
-        <v>3</v>
+        <v>4</v>
+      </c>
+      <c r="D12" s="4">
+        <v>10</v>
       </c>
       <c r="E12" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="B13" s="2">
-        <v>5</v>
+        <v>57</v>
       </c>
       <c r="C13" s="2">
-        <v>0</v>
-      </c>
-      <c r="D13" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="D13" s="4">
+        <v>12</v>
       </c>
       <c r="E13" s="2">
         <v>0</v>
@@ -1000,16 +1027,16 @@
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="2" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="B14" s="2">
-        <v>3</v>
+        <v>57</v>
       </c>
       <c r="C14" s="2">
-        <v>0</v>
-      </c>
-      <c r="D14" s="2">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D14" s="4">
+        <v>12</v>
       </c>
       <c r="E14" s="2">
         <v>0</v>
@@ -1017,33 +1044,33 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="2" t="s">
-        <v>99</v>
+        <v>18</v>
       </c>
       <c r="B15" s="2">
-        <v>8</v>
+        <v>57</v>
       </c>
       <c r="C15" s="2">
-        <v>2</v>
-      </c>
-      <c r="D15" s="2">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D15" s="4">
+        <v>12</v>
       </c>
       <c r="E15" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="2" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="B16" s="2">
-        <v>1</v>
+        <v>66</v>
       </c>
       <c r="C16" s="2">
-        <v>0</v>
-      </c>
-      <c r="D16" s="2">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="D16" s="4">
+        <v>12</v>
       </c>
       <c r="E16" s="2">
         <v>0</v>
@@ -1051,16 +1078,16 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="2" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="B17" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C17" s="2">
         <v>0</v>
       </c>
-      <c r="D17" s="2">
-        <v>0</v>
+      <c r="D17" s="4">
+        <v>12</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1068,231 +1095,231 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="2" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B18" s="2">
-        <v>0</v>
+        <v>100</v>
       </c>
       <c r="C18" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D18" s="2">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="E18" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="B19" s="2">
-        <v>106</v>
-      </c>
-      <c r="C19" s="4">
+        <v>100</v>
+      </c>
+      <c r="C19" s="2">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2">
         <v>8</v>
       </c>
-      <c r="D19" s="4">
-        <v>10</v>
-      </c>
-      <c r="E19" s="4">
-        <v>29</v>
+      <c r="E19" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B20" s="4">
-        <v>100</v>
+        <v>22</v>
+      </c>
+      <c r="B20" s="2">
+        <v>200</v>
       </c>
       <c r="C20" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D20" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="E20" s="2">
-        <v>15</v>
+        <v>0</v>
       </c>
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="2" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="B21" s="2">
-        <v>50</v>
-      </c>
-      <c r="C21" s="4">
-        <v>8</v>
-      </c>
-      <c r="D21" s="4">
-        <v>10</v>
+        <v>200</v>
+      </c>
+      <c r="C21" s="2">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2">
+        <v>9</v>
       </c>
       <c r="E21" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="22" spans="1:5">
       <c r="A22" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="B22" s="4">
-        <v>50</v>
+        <v>24</v>
+      </c>
+      <c r="B22" s="2">
+        <v>116</v>
       </c>
       <c r="C22" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D22" s="2">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="E22" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="23" spans="1:5">
       <c r="A23" s="2" t="s">
-        <v>66</v>
+        <v>25</v>
       </c>
       <c r="B23" s="2">
-        <v>50</v>
-      </c>
-      <c r="C23" s="4">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C23" s="2">
+        <v>0</v>
       </c>
       <c r="D23" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
       <c r="E23" s="2">
-        <v>14</v>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B24" s="4">
-        <v>50</v>
+        <v>26</v>
+      </c>
+      <c r="B24" s="2">
+        <v>1</v>
       </c>
       <c r="C24" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D24" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E24" s="2">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="2" t="s">
-        <v>69</v>
+        <v>27</v>
       </c>
       <c r="B25" s="2">
-        <v>50</v>
-      </c>
-      <c r="C25" s="4">
-        <v>8</v>
+        <v>3</v>
+      </c>
+      <c r="C25" s="2">
+        <v>0</v>
       </c>
       <c r="D25" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E25" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B26" s="4">
-        <v>50</v>
+        <v>28</v>
+      </c>
+      <c r="B26" s="2">
+        <v>4</v>
       </c>
       <c r="C26" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D26" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E26" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B27" s="4">
-        <v>81</v>
-      </c>
-      <c r="C27" s="4">
-        <v>8</v>
+        <v>29</v>
+      </c>
+      <c r="B27" s="2">
+        <v>5</v>
+      </c>
+      <c r="C27" s="2">
+        <v>0</v>
       </c>
       <c r="D27" s="2">
-        <v>17</v>
+        <v>1</v>
       </c>
       <c r="E27" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="28" spans="1:5">
       <c r="A28" s="2" t="s">
-        <v>72</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2">
-        <v>50</v>
+        <v>3</v>
       </c>
       <c r="C28" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="D28" s="2">
-        <v>16</v>
+        <v>0</v>
       </c>
       <c r="E28" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="4">
-        <v>50</v>
+        <v>31</v>
+      </c>
+      <c r="B29" s="2">
+        <v>2</v>
       </c>
       <c r="C29" s="2">
-        <v>21</v>
+        <v>0</v>
       </c>
       <c r="D29" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="E29" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="2" t="s">
-        <v>100</v>
+        <v>32</v>
       </c>
       <c r="B30" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C30" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D30" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="2" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B31" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C31" s="2">
         <v>0</v>
@@ -1306,10 +1333,10 @@
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B32" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C32" s="2">
         <v>0</v>
@@ -1323,10 +1350,10 @@
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="2" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B33" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C33" s="2">
         <v>0</v>
@@ -1340,10 +1367,10 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="2" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B34" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C34" s="2">
         <v>0</v>
@@ -1357,101 +1384,101 @@
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="2" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B35" s="2">
-        <v>50</v>
-      </c>
-      <c r="C35" s="4">
-        <v>8</v>
+        <v>1</v>
+      </c>
+      <c r="C35" s="2">
+        <v>0</v>
       </c>
       <c r="D35" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E35" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="B36" s="2">
-        <v>50</v>
+        <v>1</v>
       </c>
       <c r="C36" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D36" s="2">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E36" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="37" spans="1:5">
       <c r="A37" s="2" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="B37" s="2">
-        <v>50</v>
-      </c>
-      <c r="C37" s="4">
-        <v>8</v>
+        <v>2</v>
+      </c>
+      <c r="C37" s="2">
+        <v>0</v>
       </c>
       <c r="D37" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
       <c r="E37" s="2">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="2" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B38" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C38" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D38" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="E38" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="2" t="s">
-        <v>7</v>
+        <v>41</v>
       </c>
       <c r="B39" s="2">
-        <v>50</v>
-      </c>
-      <c r="C39" s="4">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="C39" s="2">
+        <v>20</v>
       </c>
       <c r="D39" s="2">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E39" s="2">
-        <v>35</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="2" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="B40" s="2">
-        <v>31</v>
+        <v>60</v>
       </c>
       <c r="C40" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D40" s="2">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="E40" s="2">
         <v>0</v>
@@ -1459,101 +1486,101 @@
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="2" t="s">
-        <v>8</v>
+        <v>43</v>
       </c>
       <c r="B41" s="2">
-        <v>50</v>
-      </c>
-      <c r="C41" s="4">
-        <v>8</v>
+        <v>60</v>
+      </c>
+      <c r="C41" s="2">
+        <v>20</v>
       </c>
       <c r="D41" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E41" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="2" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B42" s="2">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C42" s="2">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D42" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E42" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="2" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="B43" s="2">
-        <v>71</v>
-      </c>
-      <c r="C43" s="4">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="C43" s="2">
+        <v>20</v>
       </c>
       <c r="D43" s="2">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E43" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="2" t="s">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="B44" s="2">
         <v>50</v>
       </c>
       <c r="C44" s="2">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D44" s="2">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="E44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="2" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B45" s="2">
         <v>50</v>
       </c>
       <c r="C45" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="D45" s="2">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="E45" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="46" spans="1:5">
       <c r="A46" s="2" t="s">
-        <v>95</v>
+        <v>48</v>
       </c>
       <c r="B46" s="2">
         <v>50</v>
       </c>
       <c r="C46" s="2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="D46" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E46" s="2">
         <v>0</v>
@@ -1561,84 +1588,84 @@
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="2" t="s">
-        <v>96</v>
+        <v>49</v>
       </c>
       <c r="B47" s="2">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="C47" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D47" s="2">
-        <v>3</v>
+        <v>17</v>
       </c>
       <c r="E47" s="2">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="2" t="s">
-        <v>97</v>
+        <v>50</v>
       </c>
       <c r="B48" s="2">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="C48" s="2">
+        <v>12</v>
+      </c>
+      <c r="D48" s="2">
         <v>3</v>
       </c>
-      <c r="D48" s="2">
-        <v>2</v>
-      </c>
       <c r="E48" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="2" t="s">
-        <v>98</v>
+        <v>51</v>
       </c>
       <c r="B49" s="2">
-        <v>15</v>
+        <v>24</v>
       </c>
       <c r="C49" s="2">
         <v>2</v>
       </c>
       <c r="D49" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E49" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="2" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="B50" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D50" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E50" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="2" t="s">
-        <v>41</v>
+        <v>53</v>
       </c>
       <c r="B51" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C51" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D51" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E51" s="2">
         <v>0</v>
@@ -1646,33 +1673,33 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="2" t="s">
-        <v>101</v>
+        <v>54</v>
       </c>
       <c r="B52" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C52" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D52" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E52" s="2">
-        <v>67</v>
+        <v>2</v>
       </c>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="2" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B53" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C53" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D53" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E53" s="2">
         <v>2</v>
@@ -1680,50 +1707,50 @@
     </row>
     <row r="54" spans="1:5">
       <c r="A54" s="2" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="B54" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C54" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D54" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E54" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="2" t="s">
-        <v>76</v>
+        <v>57</v>
       </c>
       <c r="B55" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C55" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D55" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E55" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="2" t="s">
-        <v>77</v>
+        <v>58</v>
       </c>
       <c r="B56" s="2">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C56" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D56" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E56" s="2">
         <v>2</v>
@@ -1731,33 +1758,33 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="2" t="s">
-        <v>50</v>
+        <v>59</v>
       </c>
       <c r="B57" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C57" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D57" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E57" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="2" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="B58" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C58" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D58" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E58" s="2">
         <v>2</v>
@@ -1765,101 +1792,101 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="2" t="s">
-        <v>79</v>
+        <v>61</v>
       </c>
       <c r="B59" s="2">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C59" s="2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D59" s="2">
         <v>4</v>
       </c>
       <c r="E59" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="2" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B60" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C60" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D60" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E60" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
     </row>
     <row r="61" spans="1:5">
       <c r="A61" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="B61" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C61" s="2">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="D61" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E61" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="2" t="s">
-        <v>90</v>
+        <v>64</v>
       </c>
       <c r="B62" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C62" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D62" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E62" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="2" t="s">
-        <v>25</v>
+        <v>65</v>
       </c>
       <c r="B63" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C63" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D63" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E63" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="2" t="s">
-        <v>91</v>
+        <v>66</v>
       </c>
       <c r="B64" s="2">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="C64" s="2">
-        <v>15</v>
+        <v>2</v>
       </c>
       <c r="D64" s="2">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="E64" s="2">
         <v>2</v>
@@ -1867,169 +1894,169 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="2" t="s">
-        <v>26</v>
+        <v>67</v>
       </c>
       <c r="B65" s="2">
+        <v>10</v>
+      </c>
+      <c r="C65" s="2">
+        <v>2</v>
+      </c>
+      <c r="D65" s="2">
+        <v>4</v>
+      </c>
+      <c r="E65" s="2">
         <v>1</v>
-      </c>
-      <c r="C65" s="2">
-        <v>0</v>
-      </c>
-      <c r="D65" s="2">
-        <v>0</v>
-      </c>
-      <c r="E65" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="2" t="s">
-        <v>27</v>
+        <v>68</v>
       </c>
       <c r="B66" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C66" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D66" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E66" s="2">
-        <v>0</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="2" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="B67" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C67" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D67" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E67" s="2">
-        <v>11</v>
+        <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="2" t="s">
-        <v>43</v>
+        <v>70</v>
       </c>
       <c r="B68" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C68" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D68" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E68" s="2">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="2" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B69" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C69" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D69" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E69" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:5">
       <c r="A70" s="2" t="s">
-        <v>56</v>
+        <v>72</v>
       </c>
       <c r="B70" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C70" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D70" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E70" s="2">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:5">
       <c r="A71" s="2" t="s">
-        <v>57</v>
+        <v>73</v>
       </c>
       <c r="B71" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C71" s="2">
         <v>5</v>
       </c>
       <c r="D71" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E71" s="2">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="2" t="s">
-        <v>58</v>
+        <v>74</v>
       </c>
       <c r="B72" s="2">
-        <v>31</v>
+        <v>10</v>
       </c>
       <c r="C72" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D72" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="E72" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="2" t="s">
-        <v>59</v>
+        <v>75</v>
       </c>
       <c r="B73" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C73" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D73" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E73" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="2" t="s">
-        <v>45</v>
+        <v>76</v>
       </c>
       <c r="B74" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C74" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" s="2">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="E74" s="2">
         <v>4</v>
@@ -2037,254 +2064,254 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="2" t="s">
-        <v>10</v>
+        <v>77</v>
       </c>
       <c r="B75" s="2">
-        <v>71</v>
+        <v>10</v>
       </c>
       <c r="C75" s="2">
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="D75" s="2">
         <v>4</v>
       </c>
       <c r="E75" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="2" t="s">
-        <v>11</v>
+        <v>78</v>
       </c>
       <c r="B76" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C76" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D76" s="2">
-        <v>16</v>
+        <v>4</v>
       </c>
       <c r="E76" s="2">
-        <v>26</v>
+        <v>2</v>
       </c>
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="2" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B77" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C77" s="2">
         <v>2</v>
       </c>
       <c r="D77" s="2">
-        <v>15</v>
+        <v>4</v>
       </c>
       <c r="E77" s="2">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="2" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B78" s="2">
-        <v>50</v>
+        <v>10</v>
       </c>
       <c r="C78" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D78" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E78" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="2" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
       <c r="B79" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="C79" s="2">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="D79" s="2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E79" s="2">
-        <v>9</v>
+        <v>4</v>
       </c>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="2" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
       <c r="B80" s="2">
-        <v>92</v>
+        <v>10</v>
       </c>
       <c r="C80" s="2">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="D80" s="2">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="E80" s="2">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="2" t="s">
-        <v>94</v>
+        <v>83</v>
       </c>
       <c r="B81" s="2">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C81" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D81" s="2">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E81" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="82" spans="1:5">
       <c r="A82" s="2" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="B82" s="2">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="C82" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D82" s="2">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E82" s="2">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="83" spans="1:5">
       <c r="A83" s="2" t="s">
-        <v>12</v>
+        <v>85</v>
       </c>
       <c r="B83" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C83" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D83" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="E83" s="2">
-        <v>22</v>
+        <v>1</v>
       </c>
     </row>
     <row r="84" spans="1:5">
       <c r="A84" s="2" t="s">
-        <v>60</v>
+        <v>86</v>
       </c>
       <c r="B84" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C84" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D84" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E84" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:5">
       <c r="A85" s="2" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="B85" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C85" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D85" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="E85" s="2">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
     <row r="86" spans="1:5">
       <c r="A86" s="2" t="s">
-        <v>23</v>
+        <v>88</v>
       </c>
       <c r="B86" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C86" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D86" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E86" s="2">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="87" spans="1:5">
       <c r="A87" s="2" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="B87" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C87" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D87" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E87" s="2">
-        <v>16</v>
+        <v>2</v>
       </c>
     </row>
     <row r="88" spans="1:5">
       <c r="A88" s="2" t="s">
-        <v>61</v>
+        <v>90</v>
       </c>
       <c r="B88" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C88" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D88" s="2">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E88" s="2">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="2" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B89" s="2">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="C89" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D89" s="2">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="E89" s="2">
         <v>2</v>
@@ -2292,33 +2319,33 @@
     </row>
     <row r="90" spans="1:5">
       <c r="A90" s="2" t="s">
-        <v>46</v>
+        <v>92</v>
       </c>
       <c r="B90" s="2">
-        <v>164</v>
+        <v>10</v>
       </c>
       <c r="C90" s="2">
-        <v>35</v>
+        <v>2</v>
       </c>
       <c r="D90" s="2">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E90" s="2">
-        <v>18</v>
+        <v>9</v>
       </c>
     </row>
     <row r="91" spans="1:5">
       <c r="A91" s="2" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
       <c r="B91" s="2">
-        <v>44</v>
+        <v>10</v>
       </c>
       <c r="C91" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D91" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="E91" s="2">
         <v>1</v>
@@ -2326,30 +2353,30 @@
     </row>
     <row r="92" spans="1:5">
       <c r="A92" s="2" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="B92" s="2">
-        <v>95</v>
+        <v>10</v>
       </c>
       <c r="C92" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D92" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E92" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="93" spans="1:5">
       <c r="A93" s="2" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
       <c r="B93" s="2">
-        <v>69</v>
+        <v>10</v>
       </c>
       <c r="C93" s="2">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D93" s="2">
         <v>0</v>
@@ -2360,99 +2387,92 @@
     </row>
     <row r="94" spans="1:5">
       <c r="A94" s="2" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="B94" s="2">
-        <v>134</v>
+        <v>10</v>
       </c>
       <c r="C94" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="D94" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E94" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="2" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="B95" s="2">
-        <v>46</v>
+        <v>10</v>
       </c>
       <c r="C95" s="2">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="D95" s="2">
+        <v>2</v>
+      </c>
+      <c r="E95" s="2">
         <v>1</v>
-      </c>
-      <c r="E95" s="2">
-        <v>0</v>
       </c>
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="2" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="B96" s="2">
-        <v>106</v>
+        <v>15</v>
       </c>
       <c r="C96" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D96" s="2">
-        <v>13</v>
+        <v>0</v>
       </c>
       <c r="E96" s="2">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="2" t="s">
-        <v>28</v>
+        <v>99</v>
       </c>
       <c r="B97" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="C97" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D97" s="2">
         <v>0</v>
       </c>
       <c r="E97" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="2" t="s">
-        <v>36</v>
+        <v>100</v>
       </c>
       <c r="B98" s="2">
+        <v>93</v>
+      </c>
+      <c r="C98" s="2">
+        <v>2</v>
+      </c>
+      <c r="D98" s="2">
+        <v>1</v>
+      </c>
+      <c r="E98" s="2">
         <v>3</v>
       </c>
-      <c r="C98" s="2">
-        <v>0</v>
-      </c>
-      <c r="D98" s="2">
-        <v>0</v>
-      </c>
-      <c r="E98" s="2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:5">
-      <c r="A99" s="3"/>
-      <c r="B99" s="3"/>
-      <c r="C99" s="3"/>
-      <c r="D99" s="3"/>
-      <c r="E99" s="3"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <conditionalFormatting sqref="A1:A48 A99:A1048576">
+  <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>